<commit_message>
revision 2 and readme updates
</commit_message>
<xml_diff>
--- a/pcb/katori_BOM_PCBway.xlsx
+++ b/pcb/katori_BOM_PCBway.xlsx
@@ -134,7 +134,7 @@
     <t xml:space="preserve">Your Instructions / Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">J2</t>
+    <t xml:space="preserve">J1</t>
   </si>
   <si>
     <t xml:space="preserve">JST</t>
@@ -657,9 +657,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>664920</xdr:colOff>
+      <xdr:colOff>664560</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -673,11 +673,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="209520"/>
-          <a:ext cx="1375560" cy="374400"/>
+          <a:ext cx="1375200" cy="374040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
         </a:ln>
@@ -870,8 +871,8 @@
   </sheetPr>
   <dimension ref="A2:M26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>